<commit_message>
Lots of pre-MCC changes
</commit_message>
<xml_diff>
--- a/VEXSerialData.xlsx
+++ b/VEXSerialData.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Baud Rate</t>
   </si>
   <si>
-    <t xml:space="preserve">Bits times per byte</t>
+    <t xml:space="preserve">Bits per byte</t>
   </si>
   <si>
     <t xml:space="preserve">Item</t>
@@ -309,10 +309,10 @@
   <dimension ref="A1:D86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.14"/>

</xml_diff>